<commit_message>
intial thoughts done, continuing later
</commit_message>
<xml_diff>
--- a/Best Time to Buy and Sell Stock/Whiteboards/Solution.xlsx
+++ b/Best Time to Buy and Sell Stock/Whiteboards/Solution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Longest Palindromic Substring\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Best Time to Buy and Sell Stock\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFE340-9EA5-43EC-9B8B-09BBE60FCC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B79DF-2D7E-47B6-B86D-61D6A7D4B7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -34,6 +34,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+  <si>
+    <t>SMALLEST</t>
+  </si>
+  <si>
+    <t>LARGEST</t>
+  </si>
+  <si>
+    <t>far</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>Currently Selected Pointers</t>
+  </si>
+  <si>
+    <t>Newly considering from left pointer</t>
+  </si>
+  <si>
+    <t>Newly considering from right pointer</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>"Left" considers the left green and the left yellow for the profit margin</t>
+  </si>
+  <si>
+    <t>"Right" considers the right green and the right blue for the profit margin</t>
+  </si>
+  <si>
+    <t>"far" considers the smallest of the 2 left and the largest of the 2 right for profit margins</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,12 +86,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,10 +124,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,17 +461,460 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="D7:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AG19" sqref="AG19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>6</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
+      <c r="R17" s="3"/>
+      <c r="S17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="4"/>
+      <c r="S18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="2"/>
+      <c r="M19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>6</v>
+      </c>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
+      <c r="M20" s="1">
+        <v>-6</v>
+      </c>
+      <c r="N20" s="1">
+        <v>-2</v>
+      </c>
+      <c r="O20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7"/>
+      <c r="AC21" s="7"/>
+      <c r="AD21" s="7"/>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+    </row>
+    <row r="22" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="2"/>
+      <c r="M22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
+      <c r="AB22" s="7"/>
+      <c r="AC22" s="7"/>
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="7"/>
+      <c r="AF22" s="7"/>
+      <c r="AG22" s="7"/>
+      <c r="AH22" s="7"/>
+    </row>
+    <row r="23" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>5</v>
+      </c>
+      <c r="H23" s="1">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
+        <v>6</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+      <c r="M23" s="1">
+        <v>4</v>
+      </c>
+      <c r="N23" s="1">
+        <v>3</v>
+      </c>
+      <c r="O23" s="1">
+        <v>5</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+    </row>
+    <row r="24" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+    </row>
+    <row r="25" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+    </row>
+    <row r="26" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="2"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="2"/>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+    </row>
+    <row r="27" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>7</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>5</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>6</v>
+      </c>
+      <c r="J27" s="1">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1">
+        <v>4</v>
+      </c>
+      <c r="N27" s="1">
+        <v>3</v>
+      </c>
+      <c r="O27" s="1">
+        <v>5</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+    </row>
+    <row r="28" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6"/>
+    </row>
+    <row r="34" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="2"/>
+      <c r="N34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>100</v>
+      </c>
+      <c r="J35" s="1">
+        <v>6</v>
+      </c>
+      <c r="K35" s="1">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1">
+        <v>4</v>
+      </c>
+      <c r="O35" s="1">
+        <v>3</v>
+      </c>
+      <c r="P35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="R23:AH23"/>
+    <mergeCell ref="R22:AH22"/>
+    <mergeCell ref="R21:AH21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
returned, adjusting and developing solution
</commit_message>
<xml_diff>
--- a/Best Time to Buy and Sell Stock/Whiteboards/Solution.xlsx
+++ b/Best Time to Buy and Sell Stock/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Best Time to Buy and Sell Stock\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B79DF-2D7E-47B6-B86D-61D6A7D4B7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A43FF1A-A67C-4D80-ADF1-C64BCDC028CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>SMALLEST</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>far</t>
-  </si>
-  <si>
-    <t>stop</t>
   </si>
   <si>
     <t>Currently Selected Pointers</t>
@@ -71,6 +68,12 @@
   </si>
   <si>
     <t>"far" considers the smallest of the 2 left and the largest of the 2 right for profit margins</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>Notice the stop condition is when the newly introduced squares (yellow &amp; blue) overlap with the selected ones (greens)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,6 +143,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -461,15 +467,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="D7:AH35"/>
+  <dimension ref="D7:AI53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AG19" sqref="AG19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.7109375" style="1"/>
+    <col min="1" max="21" width="4.7109375" style="1"/>
+    <col min="22" max="22" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="4.7109375" style="1"/>
+    <col min="29" max="29" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -556,7 +566,7 @@
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -580,13 +590,13 @@
       </c>
       <c r="R17" s="3"/>
       <c r="S17" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R18" s="4"/>
       <c r="S18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,10 +605,10 @@
       <c r="I19" s="4"/>
       <c r="J19" s="2"/>
       <c r="M19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>2</v>
@@ -634,25 +644,25 @@
       </c>
     </row>
     <row r="21" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
-      <c r="AF21" s="7"/>
-      <c r="AG21" s="7"/>
-      <c r="AH21" s="7"/>
+      <c r="R21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
     </row>
     <row r="22" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="2"/>
@@ -660,33 +670,33 @@
       <c r="H22" s="4"/>
       <c r="I22" s="2"/>
       <c r="M22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-      <c r="AE22" s="7"/>
-      <c r="AF22" s="7"/>
-      <c r="AG22" s="7"/>
-      <c r="AH22" s="7"/>
+      <c r="R22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
     </row>
     <row r="23" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
@@ -716,89 +726,86 @@
       <c r="O23" s="1">
         <v>5</v>
       </c>
-      <c r="R23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
+      <c r="R23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
     </row>
     <row r="24" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
     </row>
     <row r="25" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="6"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
     </row>
     <row r="26" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
       <c r="G26" s="4"/>
       <c r="H26" s="3"/>
       <c r="I26" s="2"/>
-      <c r="K26" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="M26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="6"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="7"/>
+      <c r="AC26" s="7"/>
+      <c r="AD26" s="7"/>
+      <c r="AE26" s="7"/>
     </row>
     <row r="27" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
@@ -820,97 +827,438 @@
         <v>4</v>
       </c>
       <c r="M27" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N27" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O27" s="1">
         <v>5</v>
       </c>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7"/>
+      <c r="AC27" s="7"/>
+      <c r="AD27" s="7"/>
+      <c r="AE27" s="7"/>
     </row>
     <row r="28" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="6"/>
-      <c r="AB28" s="6"/>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-    </row>
-    <row r="34" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="2"/>
-      <c r="N34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="1">
-        <v>7</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <v>5</v>
-      </c>
-      <c r="G35" s="1">
-        <v>3</v>
-      </c>
-      <c r="H35" s="1">
-        <v>1</v>
-      </c>
-      <c r="I35" s="1">
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="7"/>
+      <c r="AD28" s="7"/>
+      <c r="AE28" s="7"/>
+    </row>
+    <row r="30" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="4"/>
+      <c r="I30" s="3"/>
+      <c r="L30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+    </row>
+    <row r="31" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="M31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3</v>
+      </c>
+      <c r="I32" s="1">
+        <v>6</v>
+      </c>
+      <c r="J32" s="1">
+        <v>4</v>
+      </c>
+      <c r="M32" s="1">
+        <v>4</v>
+      </c>
+      <c r="N32" s="1">
+        <v>3</v>
+      </c>
+      <c r="O32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="2"/>
+      <c r="N38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
         <v>100</v>
       </c>
-      <c r="J35" s="1">
-        <v>6</v>
-      </c>
-      <c r="K35" s="1">
-        <v>4</v>
-      </c>
-      <c r="N35" s="1">
-        <v>4</v>
-      </c>
-      <c r="O35" s="1">
-        <v>3</v>
-      </c>
-      <c r="P35" s="1">
-        <v>5</v>
+      <c r="J39" s="1">
+        <v>6</v>
+      </c>
+      <c r="K39" s="1">
+        <v>4</v>
+      </c>
+      <c r="N39" s="1">
+        <v>-6</v>
+      </c>
+      <c r="O39" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P39" s="1">
+        <v>5</v>
+      </c>
+      <c r="W39" s="1">
+        <v>7</v>
+      </c>
+      <c r="X39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>100</v>
+      </c>
+      <c r="AC39" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD39" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+      <c r="F41" s="3"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="2"/>
+      <c r="N41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>100</v>
+      </c>
+      <c r="J42" s="1">
+        <v>6</v>
+      </c>
+      <c r="K42" s="1">
+        <v>4</v>
+      </c>
+      <c r="N42" s="1">
+        <v>4</v>
+      </c>
+      <c r="O42" s="1">
+        <v>-94</v>
+      </c>
+      <c r="P42" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="2"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="2"/>
+      <c r="N44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="1">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>5</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1">
+        <v>100</v>
+      </c>
+      <c r="J45" s="1">
+        <v>6</v>
+      </c>
+      <c r="K45" s="1">
+        <v>4</v>
+      </c>
+      <c r="N45" s="1">
+        <v>2</v>
+      </c>
+      <c r="O45" s="1">
+        <v>99</v>
+      </c>
+      <c r="P45" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V46" s="2"/>
+      <c r="W46" s="3"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="2"/>
+      <c r="AG46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI46" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V47" s="1">
+        <v>0</v>
+      </c>
+      <c r="W47" s="1">
+        <v>1</v>
+      </c>
+      <c r="X47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AG47" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH47" s="1">
+        <v>99</v>
+      </c>
+      <c r="AI47" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="4:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="2"/>
+      <c r="N48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <v>5</v>
+      </c>
+      <c r="G49" s="1">
+        <v>3</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1">
+        <v>100</v>
+      </c>
+      <c r="J49" s="1">
+        <v>6</v>
+      </c>
+      <c r="K49" s="1">
+        <v>4</v>
+      </c>
+      <c r="N49" s="1">
+        <v>2</v>
+      </c>
+      <c r="O49" s="1">
+        <v>99</v>
+      </c>
+      <c r="P49" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="2"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="2"/>
+      <c r="N52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <v>7</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>5</v>
+      </c>
+      <c r="G53" s="1">
+        <v>3</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1">
+        <v>100</v>
+      </c>
+      <c r="J53" s="1">
+        <v>6</v>
+      </c>
+      <c r="K53" s="1">
+        <v>4</v>
+      </c>
+      <c r="N53" s="1">
+        <v>2</v>
+      </c>
+      <c r="O53" s="1">
+        <v>99</v>
+      </c>
+      <c r="P53" s="1">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="R30:AF30"/>
     <mergeCell ref="R23:AH23"/>
     <mergeCell ref="R22:AH22"/>
     <mergeCell ref="R21:AH21"/>

</xml_diff>